<commit_message>
2022.02.14 - Update GPX
</commit_message>
<xml_diff>
--- a/map/info_touring.xlsx
+++ b/map/info_touring.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/Mon Drive/Sport/CarnetSorties/Infos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j.zuchuat/Documents/GitHub/JeremyZuchuat.github.io/map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1E6837-A0D5-6B4A-B58E-C6ACC1336728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06C5968-71E3-E040-A9F3-70BD56857D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="173">
   <si>
     <t>Date</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>Gilles</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>Départ relativement tardif (9h30), en raison du retour de conditions quasi hivernales. La première section sur la piste est une véritable patinoire. Une fois Combavert atteint, le Toûno se présente a nous..mais pas pour ajourd'hui. La suite de la montée de fait tranquillement. Dans la dernière section, les rayons de midi commencent à tapper fort (et les coups de soleil qui vont avec). Au sommet, on se dirige vers le sommet secondaire, pour un pic-nic grandiose avec vue sur le Cervin. La descente se fait sans encombre; pas du grand ski, mais la bière chez JF est méritée!</t>
@@ -2866,8 +2863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="H20" zoomScale="83" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2894,10 +2891,10 @@
         <v>50</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>51</v>
@@ -2927,7 +2924,7 @@
         <v>59</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q1" s="17" t="s">
         <v>3</v>
@@ -2944,7 +2941,7 @@
     </row>
     <row r="2" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="12">
         <v>43854</v>
@@ -2953,13 +2950,13 @@
         <v>24</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G2" s="8">
         <v>2587775</v>
@@ -2981,13 +2978,13 @@
         <v>2</v>
       </c>
       <c r="M2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="O2" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="P2" s="10">
         <v>2</v>
@@ -3007,7 +3004,7 @@
     </row>
     <row r="3" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="12">
         <v>43856</v>
@@ -3016,13 +3013,13 @@
         <v>25</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="8">
         <v>2575499</v>
@@ -3047,10 +3044,10 @@
         <v>66</v>
       </c>
       <c r="N3" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="P3" s="10">
         <v>2</v>
@@ -3070,7 +3067,7 @@
     </row>
     <row r="4" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="12">
         <v>43904</v>
@@ -3079,13 +3076,13 @@
         <v>27</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G4" s="8">
         <v>2603968</v>
@@ -3110,10 +3107,10 @@
         <v>62</v>
       </c>
       <c r="N4" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="O4" s="9" t="s">
         <v>112</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>113</v>
       </c>
       <c r="P4" s="10">
         <v>1</v>
@@ -3133,22 +3130,22 @@
     </row>
     <row r="5" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="12">
         <v>44219</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G5" s="8">
         <v>2685614</v>
@@ -3170,13 +3167,13 @@
         <v>3</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N5" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="O5" s="25" t="s">
         <v>92</v>
-      </c>
-      <c r="O5" s="25" t="s">
-        <v>93</v>
       </c>
       <c r="P5" s="10">
         <v>1</v>
@@ -3196,22 +3193,22 @@
     </row>
     <row r="6" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="12">
         <v>44220</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="E6" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" s="8">
         <v>2677389</v>
@@ -3233,13 +3230,13 @@
         <v>3</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" s="25" t="s">
         <v>99</v>
-      </c>
-      <c r="O6" s="25" t="s">
-        <v>100</v>
       </c>
       <c r="P6" s="10">
         <v>2</v>
@@ -3271,10 +3268,10 @@
         <v>61</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G7" s="8">
         <v>2590400</v>
@@ -3299,7 +3296,7 @@
         <v>62</v>
       </c>
       <c r="N7" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>63</v>
@@ -3331,13 +3328,13 @@
         <v>47</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G8" s="8">
         <v>2617224</v>
@@ -3362,10 +3359,10 @@
         <v>62</v>
       </c>
       <c r="N8" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P8" s="10">
         <v>1</v>
@@ -3394,13 +3391,13 @@
         <v>48</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G9" s="8">
         <v>2600892</v>
@@ -3425,10 +3422,10 @@
         <v>66</v>
       </c>
       <c r="N9" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P9" s="10">
         <v>1</v>
@@ -3448,22 +3445,22 @@
     </row>
     <row r="10" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="12">
         <v>44275</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="E10" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="8">
         <v>2608528</v>
@@ -3485,13 +3482,13 @@
         <v>3</v>
       </c>
       <c r="M10" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N10" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="O10" s="25" t="s">
         <v>90</v>
-      </c>
-      <c r="O10" s="25" t="s">
-        <v>91</v>
       </c>
       <c r="P10" s="10">
         <v>2</v>
@@ -3511,22 +3508,22 @@
     </row>
     <row r="11" spans="1:20" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="12">
         <v>44288</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>102</v>
-      </c>
       <c r="E11" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G11" s="8">
         <v>2598348</v>
@@ -3548,13 +3545,13 @@
         <v>2</v>
       </c>
       <c r="M11" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N11" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="O11" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="O11" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="P11" s="10">
         <v>1</v>
@@ -3574,22 +3571,22 @@
     </row>
     <row r="12" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" s="12">
         <v>44291</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="E12" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G12" s="8">
         <v>2571900</v>
@@ -3611,13 +3608,13 @@
         <v>1</v>
       </c>
       <c r="M12" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="N12" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="N12" s="25" t="s">
+      <c r="O12" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="O12" s="25" t="s">
-        <v>124</v>
       </c>
       <c r="P12" s="10">
         <v>1</v>
@@ -3637,7 +3634,7 @@
     </row>
     <row r="13" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" s="12">
         <v>44297</v>
@@ -3649,10 +3646,10 @@
         <v>61</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="8">
         <v>2590499</v>
@@ -3674,13 +3671,13 @@
         <v>2</v>
       </c>
       <c r="M13" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N13" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="O13" s="25" t="s">
         <v>126</v>
-      </c>
-      <c r="O13" s="25" t="s">
-        <v>127</v>
       </c>
       <c r="P13" s="10">
         <v>1</v>
@@ -3700,22 +3697,22 @@
     </row>
     <row r="14" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" s="12">
         <v>44303</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G14" s="8">
         <v>2575020</v>
@@ -3736,13 +3733,13 @@
         <v>2</v>
       </c>
       <c r="M14" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="N14" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="O14" s="25" t="s">
         <v>130</v>
-      </c>
-      <c r="N14" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="O14" s="25" t="s">
-        <v>131</v>
       </c>
       <c r="P14" s="10">
         <v>1</v>
@@ -3762,22 +3759,22 @@
     </row>
     <row r="15" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" s="12">
         <v>44310</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>135</v>
       </c>
       <c r="G15" s="8">
         <v>2578160</v>
@@ -3799,13 +3796,13 @@
         <v>2</v>
       </c>
       <c r="M15" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O15" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P15" s="10">
         <v>1</v>
@@ -3825,22 +3822,22 @@
     </row>
     <row r="16" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B16" s="12">
         <v>44548</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="8">
         <v>2577231</v>
@@ -3862,13 +3859,13 @@
         <v>2</v>
       </c>
       <c r="M16" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="N16" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="N16" s="25" t="s">
+      <c r="O16" s="25" t="s">
         <v>143</v>
-      </c>
-      <c r="O16" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="P16" s="10">
         <v>1</v>
@@ -3888,22 +3885,22 @@
     </row>
     <row r="17" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17" s="12">
         <v>44576</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="E17" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G17" s="8">
         <v>2593948</v>
@@ -3925,13 +3922,13 @@
         <v>2</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N17" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="O17" s="25" t="s">
         <v>148</v>
-      </c>
-      <c r="O17" s="25" t="s">
-        <v>149</v>
       </c>
       <c r="P17" s="10">
         <v>1</v>
@@ -3951,22 +3948,22 @@
     </row>
     <row r="18" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18" s="12">
         <v>44583</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="F18" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G18" s="8">
         <v>2678745</v>
@@ -3988,13 +3985,13 @@
         <v>2</v>
       </c>
       <c r="M18" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="N18" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="N18" s="25" t="s">
-        <v>161</v>
-      </c>
       <c r="O18" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P18" s="10">
         <v>1</v>
@@ -4014,22 +4011,22 @@
     </row>
     <row r="19" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" s="12">
         <v>44591</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G19" s="8">
         <v>2617109</v>
@@ -4051,13 +4048,13 @@
         <v>1</v>
       </c>
       <c r="M19" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N19" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="O19" s="25" t="s">
         <v>154</v>
-      </c>
-      <c r="O19" s="25" t="s">
-        <v>155</v>
       </c>
       <c r="P19" s="10">
         <v>1</v>
@@ -4077,22 +4074,22 @@
     </row>
     <row r="20" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B20" s="12">
         <v>44598</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>163</v>
-      </c>
       <c r="E20" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G20" s="8">
         <v>2601500</v>
@@ -4117,10 +4114,10 @@
         <v>66</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O20" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P20" s="10">
         <v>1</v>
@@ -4140,22 +4137,22 @@
     </row>
     <row r="21" spans="1:20" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B21" s="12">
         <v>44604</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>171</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G21" s="8">
         <v>2554615</v>
@@ -4177,13 +4174,13 @@
         <v>3</v>
       </c>
       <c r="M21" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O21" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P21" s="10">
         <v>1</v>
@@ -4234,9 +4231,7 @@
     <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J33" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>